<commit_message>
2017-07-06: optimze assist function
</commit_message>
<xml_diff>
--- a/express/doc/package.xlsx
+++ b/express/doc/package.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>express</t>
   </si>
@@ -64,6 +64,17 @@
   </si>
   <si>
     <t>https://www.npmjs.com/package/connect-redis</t>
+  </si>
+  <si>
+    <t>gm</t>
+  </si>
+  <si>
+    <t>npm install gm --save</t>
+  </si>
+  <si>
+    <t>要预先安装GraphicMagic
+ftp://ftp.graphicsmagick.org/pub/GraphicsMagick/windows/
+安装完毕，将gm目录加入环境变量</t>
   </si>
   <si>
     <t>validator</t>
@@ -191,10 +202,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -358,36 +369,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -400,145 +543,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,152 +666,154 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1152,7 +1165,7 @@
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G15" sqref="G13:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1161,6 +1174,7 @@
     <col min="2" max="2" width="18.375" customWidth="1"/>
     <col min="3" max="3" width="30.375" customWidth="1"/>
     <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -1219,39 +1233,50 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" ht="81" spans="1:5">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1283,115 +1308,115 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2017-07-11: add test for API
</commit_message>
<xml_diff>
--- a/express/doc/package.xlsx
+++ b/express/doc/package.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12630"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
   <si>
     <t>express</t>
   </si>
@@ -75,6 +75,21 @@
     <t>要预先安装GraphicMagic
 ftp://ftp.graphicsmagick.org/pub/GraphicsMagick/windows/
 安装完毕，将gm目录加入环境变量</t>
+  </si>
+  <si>
+    <t>mocha</t>
+  </si>
+  <si>
+    <t>自动测试框架</t>
+  </si>
+  <si>
+    <t>最好全局安装，这样可以直接全局运行mocha</t>
+  </si>
+  <si>
+    <t>supertest</t>
+  </si>
+  <si>
+    <t>http测试</t>
   </si>
   <si>
     <t>validator</t>
@@ -202,10 +217,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -226,6 +241,88 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,60 +351,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,37 +367,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -369,6 +384,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -381,97 +534,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,73 +564,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,26 +578,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,6 +608,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -613,6 +628,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -636,30 +675,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -669,7 +684,7 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -678,16 +693,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -696,115 +711,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1160,17 +1175,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G13:G15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="17.125" customWidth="1"/>
     <col min="2" max="2" width="18.375" customWidth="1"/>
     <col min="3" max="3" width="30.375" customWidth="1"/>
     <col min="4" max="4" width="42.625" customWidth="1"/>
@@ -1248,35 +1263,54 @@
         <v>18</v>
       </c>
     </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1292,7 +1326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -1308,115 +1342,115 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>